<commit_message>
Implement create_user delete_user get_user_by_name login_user and update_user API
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,35 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\python-petstore-api-to-excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CDD517-9813-41E5-899F-2C285D64F6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Pets" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>user name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>theUser</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@email.com</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>theAnotherUser</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,83 +112,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,134 +419,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="17.140625" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.85546875" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="16.28515625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="18.140625" bestFit="1" customWidth="1" style="2" min="4" max="5"/>
+    <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>username</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>datetime</t>
-        </is>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>theUser</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>john@email.com</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>45917.75747646991</v>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>45918.591113935188</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>11</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>theUser</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Johna</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>john@email.com</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>45917.75796034722</v>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45918.632075499168</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>theUser</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Johnu</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>johnu@email.com</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>45917.75831208999</v>
-      </c>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
     </row>
-    <row r="5">
-      <c r="E5" s="1" t="n"/>
-    </row>
-    <row r="6">
-      <c r="E6" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="E7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="E8" s="1" t="n"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{0a217bfd-7fc6-4e23-babe-07368f99370d}" enabled="1" method="Standard" siteId="{fda9decf-e892-43ac-9d9f-1a493f9f98d0}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>